<commit_message>
Eliminação de arquivos antigos
</commit_message>
<xml_diff>
--- a/data/Simulacao Cenarios - Novo.xlsx
+++ b/data/Simulacao Cenarios - Novo.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcio Barros\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="44">
   <si>
     <t>Requisitos Usuários</t>
   </si>
@@ -150,18 +145,24 @@
   </si>
   <si>
     <t>Tempo Overwork + Exhaustion</t>
+  </si>
+  <si>
+    <t>OWH</t>
+  </si>
+  <si>
+    <t>CST</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,12 +207,12 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
+    <cellStyle name="Separador de milhares" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -269,7 +270,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -304,7 +305,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -481,36 +482,41 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:W35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="10" width="9.28515625" customWidth="1"/>
+    <col min="2" max="5" width="9.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="7" max="10" width="9.28515625" customWidth="1"/>
     <col min="11" max="11" width="9.28515625" style="3" customWidth="1"/>
     <col min="12" max="12" width="9.28515625" customWidth="1"/>
     <col min="13" max="13" width="9" customWidth="1"/>
     <col min="14" max="14" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="19" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23">
       <c r="G1">
         <v>27.8</v>
       </c>
       <c r="K1" s="4"/>
       <c r="N1" s="5"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -541,13 +547,19 @@
       <c r="Q3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R3" t="s">
+        <v>42</v>
+      </c>
+      <c r="S3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23">
       <c r="A4" t="s">
         <v>24</v>
       </c>
       <c r="B4">
-        <f>VLOOKUP(A4,$N$4:$Q$31,2,FALSE)</f>
+        <f t="shared" ref="B4:B31" si="0">VLOOKUP(A4,$N$4:$Q$31,2,FALSE)</f>
         <v>0</v>
       </c>
       <c r="C4">
@@ -596,21 +608,43 @@
       <c r="Q4">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R4">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="S4" s="6">
+        <v>433.09</v>
+      </c>
+      <c r="T4">
+        <f>(P4-O4)*8*60+R4*60*1.25</f>
+        <v>436.79999999999984</v>
+      </c>
+      <c r="U4" t="str">
+        <f>"assertEquals("&amp;SUBSTITUTE(B4,",",".")&amp;", project.getActivity("""&amp;A4&amp;""").getStartExecutionTime(), 0.1);"</f>
+        <v>assertEquals(0, project.getActivity("Requisitos Inscrições").getStartExecutionTime(), 0.1);</v>
+      </c>
+      <c r="V4" t="str">
+        <f>"assertEquals("&amp;SUBSTITUTE(C4,",",".")&amp;", project.getActivity("""&amp;A4&amp;""").getFinishingTime(), 0.1);"</f>
+        <v>assertEquals(0.83, project.getActivity("Requisitos Inscrições").getFinishingTime(), 0.1);</v>
+      </c>
+      <c r="W4" t="str">
+        <f>"assertEquals("&amp;SUBSTITUTE(D4,",",".")&amp;", project.getActivity("""&amp;A4&amp;""").getErrors(), 0.1);"</f>
+        <v>assertEquals(40.5, project.getActivity("Requisitos Inscrições").getErrors(), 0.1);</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23">
       <c r="A5" t="s">
         <v>20</v>
       </c>
       <c r="B5">
-        <f>VLOOKUP(A5,$N$4:$Q$31,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>0.83</v>
       </c>
       <c r="C5">
-        <f t="shared" ref="C5:C31" si="0">VLOOKUP(A5,$N$4:$Q$31,3,FALSE)</f>
+        <f t="shared" ref="C5:C31" si="1">VLOOKUP(A5,$N$4:$Q$31,3,FALSE)</f>
         <v>2.11</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D31" si="1">VLOOKUP(A5,$N$4:$Q$31,4,FALSE)</f>
+        <f t="shared" ref="D5:D31" si="2">VLOOKUP(A5,$N$4:$Q$31,4,FALSE)</f>
         <v>61.5</v>
       </c>
       <c r="F5">
@@ -624,19 +658,19 @@
         <v>1.26</v>
       </c>
       <c r="I5">
-        <f t="shared" ref="I5:I31" si="2">H5+ROUND(F5*G5*21/$G$1,2)</f>
+        <f t="shared" ref="I5:I31" si="3">H5+ROUND(F5*G5*21/$G$1,2)</f>
         <v>3.17</v>
       </c>
       <c r="J5" s="2" t="str">
-        <f t="shared" ref="J5:J31" si="3">IF(ABS(I5-C5)&lt;= 0.1,"ok","-")</f>
+        <f t="shared" ref="J5:J31" si="4">IF(ABS(I5-C5)&lt;= 0.1,"ok","-")</f>
         <v>-</v>
       </c>
       <c r="K5" s="3">
-        <f t="shared" ref="K5:K10" si="4">F5</f>
+        <f t="shared" ref="K5:K10" si="5">F5</f>
         <v>41</v>
       </c>
       <c r="L5" s="2" t="str">
-        <f t="shared" ref="L5:L31" si="5">IF(ABS(K5-D5)&lt;= 0.1,"ok","-")</f>
+        <f t="shared" ref="L5:L31" si="6">IF(ABS(K5-D5)&lt;= 0.1,"ok","-")</f>
         <v>-</v>
       </c>
       <c r="M5" s="2"/>
@@ -652,21 +686,39 @@
       <c r="Q5">
         <v>64.13</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R5">
+        <v>2.69</v>
+      </c>
+      <c r="S5" s="6">
+        <v>519.71</v>
+      </c>
+      <c r="U5" t="str">
+        <f t="shared" ref="U5:U31" si="7">"assertEquals("&amp;SUBSTITUTE(B5,",",".")&amp;", project.getActivity("""&amp;A5&amp;""").getStartExecutionTime(), 0.1);"</f>
+        <v>assertEquals(0.83, project.getActivity("Requisitos Turmas").getStartExecutionTime(), 0.1);</v>
+      </c>
+      <c r="V5" t="str">
+        <f t="shared" ref="V5:V31" si="8">"assertEquals("&amp;SUBSTITUTE(C5,",",".")&amp;", project.getActivity("""&amp;A5&amp;""").getFinishingTime(), 0.1);"</f>
+        <v>assertEquals(2.11, project.getActivity("Requisitos Turmas").getFinishingTime(), 0.1);</v>
+      </c>
+      <c r="W5" t="str">
+        <f t="shared" ref="W5:W31" si="9">"assertEquals("&amp;SUBSTITUTE(D5,",",".")&amp;", project.getActivity("""&amp;A5&amp;""").getErrors(), 0.1);"</f>
+        <v>assertEquals(61.5, project.getActivity("Requisitos Turmas").getErrors(), 0.1);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23">
       <c r="A6" t="s">
         <v>16</v>
       </c>
       <c r="B6">
-        <f>VLOOKUP(A6,$N$4:$Q$31,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>2.11</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.73</v>
       </c>
       <c r="D6" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="F6">
@@ -676,23 +728,23 @@
         <v>6.1728390000000001E-2</v>
       </c>
       <c r="H6">
-        <f t="shared" ref="H6:H31" si="6">I5</f>
+        <f t="shared" ref="H6:H31" si="10">I5</f>
         <v>3.17</v>
       </c>
       <c r="I6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.0999999999999996</v>
       </c>
       <c r="J6" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="K6" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
       <c r="L6" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-</v>
       </c>
       <c r="M6" s="2"/>
@@ -708,21 +760,39 @@
       <c r="Q6">
         <v>115.71</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R6">
+        <v>12.45</v>
+      </c>
+      <c r="S6" s="6">
+        <v>3391.1</v>
+      </c>
+      <c r="U6" t="str">
+        <f t="shared" si="7"/>
+        <v>assertEquals(2.11, project.getActivity("Requisitos Disciplinas").getStartExecutionTime(), 0.1);</v>
+      </c>
+      <c r="V6" t="str">
+        <f t="shared" si="8"/>
+        <v>assertEquals(2.73, project.getActivity("Requisitos Disciplinas").getFinishingTime(), 0.1);</v>
+      </c>
+      <c r="W6" t="str">
+        <f t="shared" si="9"/>
+        <v>assertEquals(30, project.getActivity("Requisitos Disciplinas").getErrors(), 0.1);</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23">
       <c r="A7" t="s">
         <v>12</v>
       </c>
       <c r="B7">
-        <f>VLOOKUP(A7,$N$4:$Q$31,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>2.73</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.44</v>
       </c>
       <c r="D7" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>34.47</v>
       </c>
       <c r="F7">
@@ -732,23 +802,23 @@
         <v>6.1728390000000001E-2</v>
       </c>
       <c r="H7">
+        <f t="shared" si="10"/>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="3"/>
+        <v>5.17</v>
+      </c>
+      <c r="J7" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+      <c r="K7" s="3">
+        <f t="shared" si="5"/>
+        <v>23</v>
+      </c>
+      <c r="L7" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="I7">
-        <f t="shared" si="2"/>
-        <v>5.17</v>
-      </c>
-      <c r="J7" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="K7" s="3">
-        <f t="shared" si="4"/>
-        <v>23</v>
-      </c>
-      <c r="L7" s="2" t="str">
-        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="M7" s="2"/>
@@ -764,21 +834,39 @@
       <c r="Q7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R7">
+        <v>21.58</v>
+      </c>
+      <c r="S7" s="6">
+        <v>4176.04</v>
+      </c>
+      <c r="U7" t="str">
+        <f t="shared" si="7"/>
+        <v>assertEquals(2.73, project.getActivity("Requisitos Aluno").getStartExecutionTime(), 0.1);</v>
+      </c>
+      <c r="V7" t="str">
+        <f t="shared" si="8"/>
+        <v>assertEquals(3.44, project.getActivity("Requisitos Aluno").getFinishingTime(), 0.1);</v>
+      </c>
+      <c r="W7" t="str">
+        <f t="shared" si="9"/>
+        <v>assertEquals(34.47, project.getActivity("Requisitos Aluno").getErrors(), 0.1);</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8">
-        <f>VLOOKUP(A8,$N$4:$Q$31,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>3.45</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.16</v>
       </c>
       <c r="D8" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>34.5</v>
       </c>
       <c r="F8">
@@ -788,23 +876,23 @@
         <v>6.1728390000000001E-2</v>
       </c>
       <c r="H8">
+        <f t="shared" si="10"/>
+        <v>5.17</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="3"/>
+        <v>6.24</v>
+      </c>
+      <c r="J8" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+      <c r="K8" s="3">
+        <f t="shared" si="5"/>
+        <v>23</v>
+      </c>
+      <c r="L8" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>5.17</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="2"/>
-        <v>6.24</v>
-      </c>
-      <c r="J8" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="K8" s="3">
-        <f t="shared" si="4"/>
-        <v>23</v>
-      </c>
-      <c r="L8" s="2" t="str">
-        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="M8" s="2"/>
@@ -820,21 +908,39 @@
       <c r="Q8">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R8">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="S8" s="6">
+        <v>481.22</v>
+      </c>
+      <c r="U8" t="str">
+        <f t="shared" si="7"/>
+        <v>assertEquals(3.45, project.getActivity("Requisitos Áreas").getStartExecutionTime(), 0.1);</v>
+      </c>
+      <c r="V8" t="str">
+        <f t="shared" si="8"/>
+        <v>assertEquals(4.16, project.getActivity("Requisitos Áreas").getFinishingTime(), 0.1);</v>
+      </c>
+      <c r="W8" t="str">
+        <f t="shared" si="9"/>
+        <v>assertEquals(34.5, project.getActivity("Requisitos Áreas").getErrors(), 0.1);</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="B9">
-        <f>VLOOKUP(A9,$N$4:$Q$31,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>4.16</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.78</v>
       </c>
       <c r="D9" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="F9">
@@ -844,23 +950,23 @@
         <v>6.1728390000000001E-2</v>
       </c>
       <c r="H9">
+        <f t="shared" si="10"/>
+        <v>6.24</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="3"/>
+        <v>7.17</v>
+      </c>
+      <c r="J9" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+      <c r="K9" s="3">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="L9" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>6.24</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="2"/>
-        <v>7.17</v>
-      </c>
-      <c r="J9" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="K9" s="3">
-        <f t="shared" si="4"/>
-        <v>20</v>
-      </c>
-      <c r="L9" s="2" t="str">
-        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="M9" s="2"/>
@@ -876,21 +982,39 @@
       <c r="Q9">
         <v>71.25</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R9">
+        <v>2.98</v>
+      </c>
+      <c r="S9" s="6">
+        <v>577.46</v>
+      </c>
+      <c r="U9" t="str">
+        <f t="shared" si="7"/>
+        <v>assertEquals(4.16, project.getActivity("Requisitos Professores").getStartExecutionTime(), 0.1);</v>
+      </c>
+      <c r="V9" t="str">
+        <f t="shared" si="8"/>
+        <v>assertEquals(4.78, project.getActivity("Requisitos Professores").getFinishingTime(), 0.1);</v>
+      </c>
+      <c r="W9" t="str">
+        <f t="shared" si="9"/>
+        <v>assertEquals(30, project.getActivity("Requisitos Professores").getErrors(), 0.1);</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23">
       <c r="A10" t="s">
         <v>0</v>
       </c>
       <c r="B10">
-        <f>VLOOKUP(A10,$N$4:$Q$31,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>4.78</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.34</v>
       </c>
       <c r="D10" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>27</v>
       </c>
       <c r="F10">
@@ -900,23 +1024,23 @@
         <v>6.1728390000000001E-2</v>
       </c>
       <c r="H10">
+        <f t="shared" si="10"/>
+        <v>7.17</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="3"/>
+        <v>8.01</v>
+      </c>
+      <c r="J10" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+      <c r="K10" s="3">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="L10" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>7.17</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="2"/>
-        <v>8.01</v>
-      </c>
-      <c r="J10" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="K10" s="3">
-        <f t="shared" si="4"/>
-        <v>18</v>
-      </c>
-      <c r="L10" s="2" t="str">
-        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="M10" s="2"/>
@@ -932,21 +1056,39 @@
       <c r="Q10">
         <v>136.52000000000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R10">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="S10" s="6">
+        <v>3849.72</v>
+      </c>
+      <c r="U10" t="str">
+        <f t="shared" si="7"/>
+        <v>assertEquals(4.78, project.getActivity("Requisitos Usuários").getStartExecutionTime(), 0.1);</v>
+      </c>
+      <c r="V10" t="str">
+        <f t="shared" si="8"/>
+        <v>assertEquals(5.34, project.getActivity("Requisitos Usuários").getFinishingTime(), 0.1);</v>
+      </c>
+      <c r="W10" t="str">
+        <f t="shared" si="9"/>
+        <v>assertEquals(27, project.getActivity("Requisitos Usuários").getErrors(), 0.1);</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23">
       <c r="A11" t="s">
         <v>25</v>
       </c>
       <c r="B11">
-        <f>VLOOKUP(A11,$N$4:$Q$31,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>5.34</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.35</v>
       </c>
       <c r="D11" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>96.19</v>
       </c>
       <c r="F11">
@@ -956,15 +1098,15 @@
         <v>7.4074000000000001E-2</v>
       </c>
       <c r="H11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>8.01</v>
       </c>
       <c r="I11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9.52</v>
       </c>
       <c r="J11" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="K11" s="3">
@@ -972,7 +1114,7 @@
         <v>60.75</v>
       </c>
       <c r="L11" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-</v>
       </c>
       <c r="M11" s="2"/>
@@ -988,21 +1130,39 @@
       <c r="Q11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R11">
+        <v>1.88</v>
+      </c>
+      <c r="S11" s="6">
+        <v>4608.79</v>
+      </c>
+      <c r="U11" t="str">
+        <f t="shared" si="7"/>
+        <v>assertEquals(5.34, project.getActivity("Projeto Inscrições").getStartExecutionTime(), 0.1);</v>
+      </c>
+      <c r="V11" t="str">
+        <f t="shared" si="8"/>
+        <v>assertEquals(6.35, project.getActivity("Projeto Inscrições").getFinishingTime(), 0.1);</v>
+      </c>
+      <c r="W11" t="str">
+        <f t="shared" si="9"/>
+        <v>assertEquals(96.19, project.getActivity("Projeto Inscrições").getErrors(), 0.1);</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23">
       <c r="A12" t="s">
         <v>21</v>
       </c>
       <c r="B12">
-        <f>VLOOKUP(A12,$N$4:$Q$31,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>6.35</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.88</v>
       </c>
       <c r="D12" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>146.06</v>
       </c>
       <c r="F12">
@@ -1012,23 +1172,23 @@
         <v>7.4074000000000001E-2</v>
       </c>
       <c r="H12">
+        <f t="shared" si="10"/>
+        <v>9.52</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="3"/>
+        <v>11.809999999999999</v>
+      </c>
+      <c r="J12" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+      <c r="K12" s="3">
+        <f t="shared" ref="K12:K17" si="11">ROUND(K5*1.25+F12,2)</f>
+        <v>92.25</v>
+      </c>
+      <c r="L12" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>9.52</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="2"/>
-        <v>11.809999999999999</v>
-      </c>
-      <c r="J12" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="K12" s="3">
-        <f t="shared" ref="K12:K17" si="7">ROUND(K5*1.25+F12,2)</f>
-        <v>92.25</v>
-      </c>
-      <c r="L12" s="2" t="str">
-        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="M12" s="2"/>
@@ -1044,21 +1204,39 @@
       <c r="Q12">
         <v>34.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R12">
+        <v>2.86</v>
+      </c>
+      <c r="S12" s="6">
+        <v>553.4</v>
+      </c>
+      <c r="U12" t="str">
+        <f t="shared" si="7"/>
+        <v>assertEquals(6.35, project.getActivity("Projeto Turmas").getStartExecutionTime(), 0.1);</v>
+      </c>
+      <c r="V12" t="str">
+        <f t="shared" si="8"/>
+        <v>assertEquals(7.88, project.getActivity("Projeto Turmas").getFinishingTime(), 0.1);</v>
+      </c>
+      <c r="W12" t="str">
+        <f t="shared" si="9"/>
+        <v>assertEquals(146.06, project.getActivity("Projeto Turmas").getErrors(), 0.1);</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23">
       <c r="A13" t="s">
         <v>17</v>
       </c>
       <c r="B13">
-        <f>VLOOKUP(A13,$N$4:$Q$31,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>7.88</v>
       </c>
       <c r="C13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.6199999999999992</v>
       </c>
       <c r="D13" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>71.25</v>
       </c>
       <c r="F13">
@@ -1068,23 +1246,23 @@
         <v>7.4074000000000001E-2</v>
       </c>
       <c r="H13">
+        <f t="shared" si="10"/>
+        <v>11.809999999999999</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="3"/>
+        <v>12.93</v>
+      </c>
+      <c r="J13" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+      <c r="K13" s="3">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="L13" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>11.809999999999999</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="2"/>
-        <v>12.93</v>
-      </c>
-      <c r="J13" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="K13" s="3">
-        <f t="shared" si="7"/>
-        <v>45</v>
-      </c>
-      <c r="L13" s="2" t="str">
-        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="M13" s="2"/>
@@ -1100,21 +1278,39 @@
       <c r="Q13">
         <v>81.94</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R13">
+        <v>3.43</v>
+      </c>
+      <c r="S13" s="6">
+        <v>664.08</v>
+      </c>
+      <c r="U13" t="str">
+        <f t="shared" si="7"/>
+        <v>assertEquals(7.88, project.getActivity("Projeto Disciplinas").getStartExecutionTime(), 0.1);</v>
+      </c>
+      <c r="V13" t="str">
+        <f t="shared" si="8"/>
+        <v>assertEquals(8.62, project.getActivity("Projeto Disciplinas").getFinishingTime(), 0.1);</v>
+      </c>
+      <c r="W13" t="str">
+        <f t="shared" si="9"/>
+        <v>assertEquals(71.25, project.getActivity("Projeto Disciplinas").getErrors(), 0.1);</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14">
-        <f>VLOOKUP(A14,$N$4:$Q$31,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>8.6199999999999992</v>
       </c>
       <c r="C14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.48</v>
       </c>
       <c r="D14" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>81.900000000000006</v>
       </c>
       <c r="F14">
@@ -1124,23 +1320,23 @@
         <v>7.4074000000000001E-2</v>
       </c>
       <c r="H14">
+        <f t="shared" si="10"/>
+        <v>12.93</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="3"/>
+        <v>14.219999999999999</v>
+      </c>
+      <c r="J14" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+      <c r="K14" s="3">
+        <f t="shared" si="11"/>
+        <v>51.75</v>
+      </c>
+      <c r="L14" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>12.93</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="2"/>
-        <v>14.219999999999999</v>
-      </c>
-      <c r="J14" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="K14" s="3">
-        <f t="shared" si="7"/>
-        <v>51.75</v>
-      </c>
-      <c r="L14" s="2" t="str">
-        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="M14" s="2"/>
@@ -1156,21 +1352,39 @@
       <c r="Q14">
         <v>157</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R14">
+        <v>22.88</v>
+      </c>
+      <c r="S14" s="6">
+        <v>4427.18</v>
+      </c>
+      <c r="U14" t="str">
+        <f t="shared" si="7"/>
+        <v>assertEquals(8.62, project.getActivity("Projeto Aluno").getStartExecutionTime(), 0.1);</v>
+      </c>
+      <c r="V14" t="str">
+        <f t="shared" si="8"/>
+        <v>assertEquals(9.48, project.getActivity("Projeto Aluno").getFinishingTime(), 0.1);</v>
+      </c>
+      <c r="W14" t="str">
+        <f t="shared" si="9"/>
+        <v>assertEquals(81.9, project.getActivity("Projeto Aluno").getErrors(), 0.1);</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23">
       <c r="A15" t="s">
         <v>9</v>
       </c>
       <c r="B15">
-        <f>VLOOKUP(A15,$N$4:$Q$31,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>9.48</v>
       </c>
       <c r="C15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10.34</v>
       </c>
       <c r="D15" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>81.94</v>
       </c>
       <c r="F15">
@@ -1180,23 +1394,23 @@
         <v>7.4074000000000001E-2</v>
       </c>
       <c r="H15">
+        <f t="shared" si="10"/>
+        <v>14.219999999999999</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="3"/>
+        <v>15.509999999999998</v>
+      </c>
+      <c r="J15" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+      <c r="K15" s="3">
+        <f t="shared" si="11"/>
+        <v>51.75</v>
+      </c>
+      <c r="L15" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>14.219999999999999</v>
-      </c>
-      <c r="I15">
-        <f t="shared" si="2"/>
-        <v>15.509999999999998</v>
-      </c>
-      <c r="J15" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="K15" s="3">
-        <f t="shared" si="7"/>
-        <v>51.75</v>
-      </c>
-      <c r="L15" s="2" t="str">
-        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="M15" s="2"/>
@@ -1212,21 +1426,39 @@
       <c r="Q15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15" s="6">
+        <v>5270.87</v>
+      </c>
+      <c r="U15" t="str">
+        <f t="shared" si="7"/>
+        <v>assertEquals(9.48, project.getActivity("Projeto Áreas").getStartExecutionTime(), 0.1);</v>
+      </c>
+      <c r="V15" t="str">
+        <f t="shared" si="8"/>
+        <v>assertEquals(10.34, project.getActivity("Projeto Áreas").getFinishingTime(), 0.1);</v>
+      </c>
+      <c r="W15" t="str">
+        <f t="shared" si="9"/>
+        <v>assertEquals(81.94, project.getActivity("Projeto Áreas").getErrors(), 0.1);</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23">
       <c r="A16" t="s">
         <v>5</v>
       </c>
       <c r="B16">
-        <f>VLOOKUP(A16,$N$4:$Q$31,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>10.34</v>
       </c>
       <c r="C16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11.09</v>
       </c>
       <c r="D16" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>71.25</v>
       </c>
       <c r="F16">
@@ -1236,23 +1468,23 @@
         <v>7.4074000000000001E-2</v>
       </c>
       <c r="H16">
+        <f t="shared" si="10"/>
+        <v>15.509999999999998</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="3"/>
+        <v>16.63</v>
+      </c>
+      <c r="J16" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+      <c r="K16" s="3">
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="L16" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>15.509999999999998</v>
-      </c>
-      <c r="I16">
-        <f t="shared" si="2"/>
-        <v>16.63</v>
-      </c>
-      <c r="J16" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="K16" s="3">
-        <f t="shared" si="7"/>
-        <v>45</v>
-      </c>
-      <c r="L16" s="2" t="str">
-        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="M16" s="2"/>
@@ -1268,21 +1500,39 @@
       <c r="Q16">
         <v>34.47</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R16">
+        <v>2.86</v>
+      </c>
+      <c r="S16" s="6">
+        <v>552.95000000000005</v>
+      </c>
+      <c r="U16" t="str">
+        <f t="shared" si="7"/>
+        <v>assertEquals(10.34, project.getActivity("Projeto Professores").getStartExecutionTime(), 0.1);</v>
+      </c>
+      <c r="V16" t="str">
+        <f t="shared" si="8"/>
+        <v>assertEquals(11.09, project.getActivity("Projeto Professores").getFinishingTime(), 0.1);</v>
+      </c>
+      <c r="W16" t="str">
+        <f t="shared" si="9"/>
+        <v>assertEquals(71.25, project.getActivity("Projeto Professores").getErrors(), 0.1);</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23">
       <c r="A17" t="s">
         <v>1</v>
       </c>
       <c r="B17">
-        <f>VLOOKUP(A17,$N$4:$Q$31,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>11.09</v>
       </c>
       <c r="C17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11.76</v>
       </c>
       <c r="D17" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>64.13</v>
       </c>
       <c r="F17">
@@ -1292,23 +1542,23 @@
         <v>7.4074000000000001E-2</v>
       </c>
       <c r="H17">
+        <f t="shared" si="10"/>
+        <v>16.63</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="3"/>
+        <v>17.64</v>
+      </c>
+      <c r="J17" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+      <c r="K17" s="3">
+        <f t="shared" si="11"/>
+        <v>40.5</v>
+      </c>
+      <c r="L17" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>16.63</v>
-      </c>
-      <c r="I17">
-        <f t="shared" si="2"/>
-        <v>17.64</v>
-      </c>
-      <c r="J17" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="K17" s="3">
-        <f t="shared" si="7"/>
-        <v>40.5</v>
-      </c>
-      <c r="L17" s="2" t="str">
-        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="M17" s="2"/>
@@ -1324,21 +1574,39 @@
       <c r="Q17">
         <v>81.900000000000006</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R17">
+        <v>3.43</v>
+      </c>
+      <c r="S17" s="6">
+        <v>664.08</v>
+      </c>
+      <c r="U17" t="str">
+        <f t="shared" si="7"/>
+        <v>assertEquals(11.09, project.getActivity("Projeto Usuários").getStartExecutionTime(), 0.1);</v>
+      </c>
+      <c r="V17" t="str">
+        <f t="shared" si="8"/>
+        <v>assertEquals(11.76, project.getActivity("Projeto Usuários").getFinishingTime(), 0.1);</v>
+      </c>
+      <c r="W17" t="str">
+        <f t="shared" si="9"/>
+        <v>assertEquals(64.13, project.getActivity("Projeto Usuários").getErrors(), 0.1);</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23">
       <c r="A18" t="s">
         <v>26</v>
       </c>
       <c r="B18">
-        <f>VLOOKUP(A18,$N$4:$Q$31,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>11.76</v>
       </c>
       <c r="C18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18.47</v>
       </c>
       <c r="D18" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>184.3</v>
       </c>
       <c r="F18">
@@ -1348,15 +1616,15 @@
         <v>0.49382710000000002</v>
       </c>
       <c r="H18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>17.64</v>
       </c>
       <c r="I18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>27.71</v>
       </c>
       <c r="J18" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="K18" s="3">
@@ -1364,7 +1632,7 @@
         <v>107.8</v>
       </c>
       <c r="L18" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-</v>
       </c>
       <c r="M18" s="2"/>
@@ -1380,21 +1648,39 @@
       <c r="Q18">
         <v>156.94</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R18">
+        <v>22.88</v>
+      </c>
+      <c r="S18" s="6">
+        <v>4427.18</v>
+      </c>
+      <c r="U18" t="str">
+        <f t="shared" si="7"/>
+        <v>assertEquals(11.76, project.getActivity("Codificacao Inscrições").getStartExecutionTime(), 0.1);</v>
+      </c>
+      <c r="V18" t="str">
+        <f t="shared" si="8"/>
+        <v>assertEquals(18.47, project.getActivity("Codificacao Inscrições").getFinishingTime(), 0.1);</v>
+      </c>
+      <c r="W18" t="str">
+        <f t="shared" si="9"/>
+        <v>assertEquals(184.3, project.getActivity("Codificacao Inscrições").getErrors(), 0.1);</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23">
       <c r="A19" t="s">
         <v>22</v>
       </c>
       <c r="B19">
-        <f>VLOOKUP(A19,$N$4:$Q$31,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>18.47</v>
       </c>
       <c r="C19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>33.07</v>
       </c>
       <c r="D19" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>233.65</v>
       </c>
       <c r="F19">
@@ -1404,23 +1690,23 @@
         <v>0.49382710000000002</v>
       </c>
       <c r="H19">
+        <f t="shared" si="10"/>
+        <v>27.71</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="J19" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+      <c r="K19" s="3">
+        <f t="shared" ref="K19:K24" si="12">ROUND(K12*1.33+F19,2)</f>
+        <v>163.69</v>
+      </c>
+      <c r="L19" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>27.71</v>
-      </c>
-      <c r="I19">
-        <f t="shared" si="2"/>
-        <v>43</v>
-      </c>
-      <c r="J19" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="K19" s="3">
-        <f t="shared" ref="K19:K24" si="8">ROUND(K12*1.33+F19,2)</f>
-        <v>163.69</v>
-      </c>
-      <c r="L19" s="2" t="str">
-        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="M19" s="2"/>
@@ -1436,21 +1722,39 @@
       <c r="Q19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R19">
+        <v>28.83</v>
+      </c>
+      <c r="S19" s="6">
+        <v>5658.13</v>
+      </c>
+      <c r="U19" t="str">
+        <f t="shared" si="7"/>
+        <v>assertEquals(18.47, project.getActivity("Codificacao Turmas").getStartExecutionTime(), 0.1);</v>
+      </c>
+      <c r="V19" t="str">
+        <f t="shared" si="8"/>
+        <v>assertEquals(33.07, project.getActivity("Codificacao Turmas").getFinishingTime(), 0.1);</v>
+      </c>
+      <c r="W19" t="str">
+        <f t="shared" si="9"/>
+        <v>assertEquals(233.65, project.getActivity("Codificacao Turmas").getErrors(), 0.1);</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20">
-        <f>VLOOKUP(A20,$N$4:$Q$31,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>33.07</v>
       </c>
       <c r="C20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40.31</v>
       </c>
       <c r="D20" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>112.74</v>
       </c>
       <c r="F20">
@@ -1460,23 +1764,23 @@
         <v>0.49382710000000002</v>
       </c>
       <c r="H20">
+        <f t="shared" si="10"/>
+        <v>43</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="3"/>
+        <v>50.46</v>
+      </c>
+      <c r="J20" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+      <c r="K20" s="3">
+        <f t="shared" si="12"/>
+        <v>79.849999999999994</v>
+      </c>
+      <c r="L20" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>43</v>
-      </c>
-      <c r="I20">
-        <f t="shared" si="2"/>
-        <v>50.46</v>
-      </c>
-      <c r="J20" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="K20" s="3">
-        <f t="shared" si="8"/>
-        <v>79.849999999999994</v>
-      </c>
-      <c r="L20" s="2" t="str">
-        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="M20" s="2"/>
@@ -1492,21 +1796,39 @@
       <c r="Q20">
         <v>30</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R20">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="S20" s="6">
+        <v>481.22</v>
+      </c>
+      <c r="U20" t="str">
+        <f t="shared" si="7"/>
+        <v>assertEquals(33.07, project.getActivity("Codificacao Disciplinas").getStartExecutionTime(), 0.1);</v>
+      </c>
+      <c r="V20" t="str">
+        <f t="shared" si="8"/>
+        <v>assertEquals(40.31, project.getActivity("Codificacao Disciplinas").getFinishingTime(), 0.1);</v>
+      </c>
+      <c r="W20" t="str">
+        <f t="shared" si="9"/>
+        <v>assertEquals(112.74, project.getActivity("Codificacao Disciplinas").getErrors(), 0.1);</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23">
       <c r="A21" t="s">
         <v>14</v>
       </c>
       <c r="B21">
-        <f>VLOOKUP(A21,$N$4:$Q$31,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>40.31</v>
       </c>
       <c r="C21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>46.03</v>
       </c>
       <c r="D21" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>156.94</v>
       </c>
       <c r="F21">
@@ -1516,23 +1838,23 @@
         <v>0.49382710000000002</v>
       </c>
       <c r="H21">
+        <f t="shared" si="10"/>
+        <v>50.46</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="3"/>
+        <v>59.04</v>
+      </c>
+      <c r="J21" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+      <c r="K21" s="3">
+        <f t="shared" si="12"/>
+        <v>91.83</v>
+      </c>
+      <c r="L21" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>50.46</v>
-      </c>
-      <c r="I21">
-        <f t="shared" si="2"/>
-        <v>59.04</v>
-      </c>
-      <c r="J21" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="K21" s="3">
-        <f t="shared" si="8"/>
-        <v>91.83</v>
-      </c>
-      <c r="L21" s="2" t="str">
-        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="M21" s="2"/>
@@ -1548,21 +1870,39 @@
       <c r="Q21">
         <v>71.25</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R21">
+        <v>2.98</v>
+      </c>
+      <c r="S21" s="6">
+        <v>577.46</v>
+      </c>
+      <c r="U21" t="str">
+        <f t="shared" si="7"/>
+        <v>assertEquals(40.31, project.getActivity("Codificacao Aluno").getStartExecutionTime(), 0.1);</v>
+      </c>
+      <c r="V21" t="str">
+        <f t="shared" si="8"/>
+        <v>assertEquals(46.03, project.getActivity("Codificacao Aluno").getFinishingTime(), 0.1);</v>
+      </c>
+      <c r="W21" t="str">
+        <f t="shared" si="9"/>
+        <v>assertEquals(156.94, project.getActivity("Codificacao Aluno").getErrors(), 0.1);</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23">
       <c r="A22" t="s">
         <v>10</v>
       </c>
       <c r="B22">
-        <f>VLOOKUP(A22,$N$4:$Q$31,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>46.03</v>
       </c>
       <c r="C22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>51.75</v>
       </c>
       <c r="D22" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>157</v>
       </c>
       <c r="F22">
@@ -1572,23 +1912,23 @@
         <v>0.49382710000000002</v>
       </c>
       <c r="H22">
+        <f t="shared" si="10"/>
+        <v>59.04</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="3"/>
+        <v>67.62</v>
+      </c>
+      <c r="J22" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+      <c r="K22" s="3">
+        <f t="shared" si="12"/>
+        <v>91.83</v>
+      </c>
+      <c r="L22" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>59.04</v>
-      </c>
-      <c r="I22">
-        <f t="shared" si="2"/>
-        <v>67.62</v>
-      </c>
-      <c r="J22" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="K22" s="3">
-        <f t="shared" si="8"/>
-        <v>91.83</v>
-      </c>
-      <c r="L22" s="2" t="str">
-        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="M22" s="2"/>
@@ -1604,21 +1944,39 @@
       <c r="Q22">
         <v>112.74</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R22">
+        <v>1.78</v>
+      </c>
+      <c r="S22" s="6">
+        <v>3605.1</v>
+      </c>
+      <c r="U22" t="str">
+        <f t="shared" si="7"/>
+        <v>assertEquals(46.03, project.getActivity("Codificacao Áreas").getStartExecutionTime(), 0.1);</v>
+      </c>
+      <c r="V22" t="str">
+        <f t="shared" si="8"/>
+        <v>assertEquals(51.75, project.getActivity("Codificacao Áreas").getFinishingTime(), 0.1);</v>
+      </c>
+      <c r="W22" t="str">
+        <f t="shared" si="9"/>
+        <v>assertEquals(157, project.getActivity("Codificacao Áreas").getErrors(), 0.1);</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23">
       <c r="A23" t="s">
         <v>6</v>
       </c>
       <c r="B23">
-        <f>VLOOKUP(A23,$N$4:$Q$31,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>51.75</v>
       </c>
       <c r="C23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>56.72</v>
       </c>
       <c r="D23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>136.52000000000001</v>
       </c>
       <c r="F23">
@@ -1628,23 +1986,23 @@
         <v>0.49382710000000002</v>
       </c>
       <c r="H23">
+        <f t="shared" si="10"/>
+        <v>67.62</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="3"/>
+        <v>75.08</v>
+      </c>
+      <c r="J23" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+      <c r="K23" s="3">
+        <f t="shared" si="12"/>
+        <v>79.849999999999994</v>
+      </c>
+      <c r="L23" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>67.62</v>
-      </c>
-      <c r="I23">
-        <f t="shared" si="2"/>
-        <v>75.08</v>
-      </c>
-      <c r="J23" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="K23" s="3">
-        <f t="shared" si="8"/>
-        <v>79.849999999999994</v>
-      </c>
-      <c r="L23" s="2" t="str">
-        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="M23" s="2"/>
@@ -1660,21 +2018,39 @@
       <c r="Q23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R23">
+        <v>21.03</v>
+      </c>
+      <c r="S23" s="6">
+        <v>4068.95</v>
+      </c>
+      <c r="U23" t="str">
+        <f t="shared" si="7"/>
+        <v>assertEquals(51.75, project.getActivity("Codificacao Professores").getStartExecutionTime(), 0.1);</v>
+      </c>
+      <c r="V23" t="str">
+        <f t="shared" si="8"/>
+        <v>assertEquals(56.72, project.getActivity("Codificacao Professores").getFinishingTime(), 0.1);</v>
+      </c>
+      <c r="W23" t="str">
+        <f t="shared" si="9"/>
+        <v>assertEquals(136.52, project.getActivity("Codificacao Professores").getErrors(), 0.1);</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23">
       <c r="A24" t="s">
         <v>2</v>
       </c>
       <c r="B24">
-        <f>VLOOKUP(A24,$N$4:$Q$31,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>56.72</v>
       </c>
       <c r="C24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>61.88</v>
       </c>
       <c r="D24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>115.71</v>
       </c>
       <c r="F24">
@@ -1684,23 +2060,23 @@
         <v>0.49382710000000002</v>
       </c>
       <c r="H24">
+        <f t="shared" si="10"/>
+        <v>75.08</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="3"/>
+        <v>81.789999999999992</v>
+      </c>
+      <c r="J24" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+      <c r="K24" s="3">
+        <f t="shared" si="12"/>
+        <v>71.87</v>
+      </c>
+      <c r="L24" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>75.08</v>
-      </c>
-      <c r="I24">
-        <f t="shared" si="2"/>
-        <v>81.789999999999992</v>
-      </c>
-      <c r="J24" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="K24" s="3">
-        <f t="shared" si="8"/>
-        <v>71.87</v>
-      </c>
-      <c r="L24" s="2" t="str">
-        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="M24" s="2"/>
@@ -1716,345 +2092,471 @@
       <c r="Q24">
         <v>61.5</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R24">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="S24" s="6">
+        <v>986.49</v>
+      </c>
+      <c r="U24" t="str">
+        <f t="shared" si="7"/>
+        <v>assertEquals(56.72, project.getActivity("Codificacao Usuários").getStartExecutionTime(), 0.1);</v>
+      </c>
+      <c r="V24" t="str">
+        <f t="shared" si="8"/>
+        <v>assertEquals(61.88, project.getActivity("Codificacao Usuários").getFinishingTime(), 0.1);</v>
+      </c>
+      <c r="W24" t="str">
+        <f t="shared" si="9"/>
+        <v>assertEquals(115.71, project.getActivity("Codificacao Usuários").getErrors(), 0.1);</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23">
       <c r="A25" t="s">
         <v>27</v>
       </c>
       <c r="B25">
-        <f>VLOOKUP(A25,$N$4:$Q$31,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>61.88</v>
       </c>
       <c r="C25">
+        <f t="shared" si="1"/>
+        <v>74.77</v>
+      </c>
+      <c r="D25" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>27</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0.37037050999999993</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="10"/>
+        <v>81.789999999999992</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="3"/>
+        <v>89.339999999999989</v>
+      </c>
+      <c r="J25" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+      <c r="K25" s="3">
+        <v>0</v>
+      </c>
+      <c r="L25" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>ok</v>
+      </c>
+      <c r="N25" t="s">
+        <v>21</v>
+      </c>
+      <c r="O25">
+        <v>6.35</v>
+      </c>
+      <c r="P25">
+        <v>7.88</v>
+      </c>
+      <c r="Q25">
+        <v>146.06</v>
+      </c>
+      <c r="R25">
+        <v>6.12</v>
+      </c>
+      <c r="S25" s="6">
+        <v>1183.79</v>
+      </c>
+      <c r="U25" t="str">
+        <f t="shared" si="7"/>
+        <v>assertEquals(61.88, project.getActivity("Testes Inscrições").getStartExecutionTime(), 0.1);</v>
+      </c>
+      <c r="V25" t="str">
+        <f t="shared" si="8"/>
+        <v>assertEquals(74.77, project.getActivity("Testes Inscrições").getFinishingTime(), 0.1);</v>
+      </c>
+      <c r="W25" t="str">
+        <f t="shared" si="9"/>
+        <v>assertEquals(0, project.getActivity("Testes Inscrições").getErrors(), 0.1);</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23">
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26">
         <f t="shared" si="0"/>
         <v>74.77</v>
       </c>
-      <c r="D25" s="3">
+      <c r="C26">
         <f t="shared" si="1"/>
+        <v>87.35</v>
+      </c>
+      <c r="D26" s="3">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F25">
-        <v>27</v>
-      </c>
-      <c r="G25" s="1">
+      <c r="F26">
+        <v>41</v>
+      </c>
+      <c r="G26" s="1">
         <v>0.37037050999999993</v>
       </c>
-      <c r="H25">
+      <c r="H26">
+        <f t="shared" si="10"/>
+        <v>89.339999999999989</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="3"/>
+        <v>100.80999999999999</v>
+      </c>
+      <c r="J26" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+      <c r="K26" s="3">
+        <v>0</v>
+      </c>
+      <c r="L26" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>81.789999999999992</v>
-      </c>
-      <c r="I25">
-        <f t="shared" si="2"/>
-        <v>89.339999999999989</v>
-      </c>
-      <c r="J25" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="K25" s="3">
-        <v>0</v>
-      </c>
-      <c r="L25" s="2" t="str">
-        <f t="shared" si="5"/>
         <v>ok</v>
       </c>
-      <c r="N25" t="s">
-        <v>21</v>
-      </c>
-      <c r="O25">
-        <v>6.35</v>
-      </c>
-      <c r="P25">
-        <v>7.88</v>
-      </c>
-      <c r="Q25">
-        <v>146.06</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>23</v>
-      </c>
-      <c r="B26">
-        <f>VLOOKUP(A26,$N$4:$Q$31,2,FALSE)</f>
-        <v>74.77</v>
-      </c>
-      <c r="C26">
+      <c r="N26" t="s">
+        <v>22</v>
+      </c>
+      <c r="O26">
+        <v>18.47</v>
+      </c>
+      <c r="P26">
+        <v>33.07</v>
+      </c>
+      <c r="Q26">
+        <v>233.65</v>
+      </c>
+      <c r="R26">
+        <v>5.57</v>
+      </c>
+      <c r="S26" s="6">
+        <v>7416.54</v>
+      </c>
+      <c r="U26" t="str">
+        <f t="shared" si="7"/>
+        <v>assertEquals(74.77, project.getActivity("Testes Turmas").getStartExecutionTime(), 0.1);</v>
+      </c>
+      <c r="V26" t="str">
+        <f t="shared" si="8"/>
+        <v>assertEquals(87.35, project.getActivity("Testes Turmas").getFinishingTime(), 0.1);</v>
+      </c>
+      <c r="W26" t="str">
+        <f t="shared" si="9"/>
+        <v>assertEquals(0, project.getActivity("Testes Turmas").getErrors(), 0.1);</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23">
+      <c r="A27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27">
         <f t="shared" si="0"/>
         <v>87.35</v>
       </c>
-      <c r="D26" s="3">
+      <c r="C27">
         <f t="shared" si="1"/>
+        <v>92.61</v>
+      </c>
+      <c r="D27" s="3">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F26">
-        <v>41</v>
-      </c>
-      <c r="G26" s="1">
+      <c r="F27">
+        <v>20</v>
+      </c>
+      <c r="G27" s="1">
         <v>0.37037050999999993</v>
       </c>
-      <c r="H26">
+      <c r="H27">
+        <f t="shared" si="10"/>
+        <v>100.80999999999999</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="3"/>
+        <v>106.40999999999998</v>
+      </c>
+      <c r="J27" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+      <c r="K27" s="3">
+        <v>0</v>
+      </c>
+      <c r="L27" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>89.339999999999989</v>
-      </c>
-      <c r="I26">
-        <f t="shared" si="2"/>
-        <v>100.80999999999999</v>
-      </c>
-      <c r="J26" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="K26" s="3">
+        <v>ok</v>
+      </c>
+      <c r="N27" t="s">
+        <v>23</v>
+      </c>
+      <c r="O27">
+        <v>74.77</v>
+      </c>
+      <c r="P27">
+        <v>87.35</v>
+      </c>
+      <c r="Q27">
         <v>0</v>
       </c>
-      <c r="L26" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>ok</v>
-      </c>
-      <c r="N26" t="s">
-        <v>22</v>
-      </c>
-      <c r="O26">
-        <v>18.47</v>
-      </c>
-      <c r="P26">
-        <v>33.07</v>
-      </c>
-      <c r="Q26">
-        <v>233.65</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27">
-        <f>VLOOKUP(A27,$N$4:$Q$31,2,FALSE)</f>
-        <v>87.35</v>
-      </c>
-      <c r="C27">
+      <c r="R27">
+        <v>30.1</v>
+      </c>
+      <c r="S27" s="6">
+        <v>8250.92</v>
+      </c>
+      <c r="U27" t="str">
+        <f t="shared" si="7"/>
+        <v>assertEquals(87.35, project.getActivity("Testes Disciplinas").getStartExecutionTime(), 0.1);</v>
+      </c>
+      <c r="V27" t="str">
+        <f t="shared" si="8"/>
+        <v>assertEquals(92.61, project.getActivity("Testes Disciplinas").getFinishingTime(), 0.1);</v>
+      </c>
+      <c r="W27" t="str">
+        <f t="shared" si="9"/>
+        <v>assertEquals(0, project.getActivity("Testes Disciplinas").getErrors(), 0.1);</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23">
+      <c r="A28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28">
         <f t="shared" si="0"/>
         <v>92.61</v>
       </c>
-      <c r="D27" s="3">
+      <c r="C28">
         <f t="shared" si="1"/>
+        <v>99.98</v>
+      </c>
+      <c r="D28" s="3">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F27">
-        <v>20</v>
-      </c>
-      <c r="G27" s="1">
+      <c r="F28">
+        <v>23</v>
+      </c>
+      <c r="G28" s="1">
         <v>0.37037050999999993</v>
       </c>
-      <c r="H27">
+      <c r="H28">
+        <f t="shared" si="10"/>
+        <v>106.40999999999998</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="3"/>
+        <v>112.83999999999997</v>
+      </c>
+      <c r="J28" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+      <c r="K28" s="3">
+        <v>0</v>
+      </c>
+      <c r="L28" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>100.80999999999999</v>
-      </c>
-      <c r="I27">
-        <f t="shared" si="2"/>
-        <v>106.40999999999998</v>
-      </c>
-      <c r="J27" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="K27" s="3">
+        <v>ok</v>
+      </c>
+      <c r="N28" t="s">
+        <v>24</v>
+      </c>
+      <c r="O28">
         <v>0</v>
       </c>
-      <c r="L27" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>ok</v>
-      </c>
-      <c r="N27" t="s">
-        <v>23</v>
-      </c>
-      <c r="O27">
-        <v>74.77</v>
-      </c>
-      <c r="P27">
-        <v>87.35</v>
-      </c>
-      <c r="Q27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>15</v>
-      </c>
-      <c r="B28">
-        <f>VLOOKUP(A28,$N$4:$Q$31,2,FALSE)</f>
-        <v>92.61</v>
-      </c>
-      <c r="C28">
+      <c r="P28">
+        <v>0.83</v>
+      </c>
+      <c r="Q28">
+        <v>40.5</v>
+      </c>
+      <c r="R28">
+        <v>3.36</v>
+      </c>
+      <c r="S28" s="6">
+        <v>649.64</v>
+      </c>
+      <c r="U28" t="str">
+        <f t="shared" si="7"/>
+        <v>assertEquals(92.61, project.getActivity("Testes Aluno").getStartExecutionTime(), 0.1);</v>
+      </c>
+      <c r="V28" t="str">
+        <f t="shared" si="8"/>
+        <v>assertEquals(99.98, project.getActivity("Testes Aluno").getFinishingTime(), 0.1);</v>
+      </c>
+      <c r="W28" t="str">
+        <f t="shared" si="9"/>
+        <v>assertEquals(0, project.getActivity("Testes Aluno").getErrors(), 0.1);</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23">
+      <c r="A29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29">
         <f t="shared" si="0"/>
         <v>99.98</v>
       </c>
-      <c r="D28" s="3">
+      <c r="C29">
         <f t="shared" si="1"/>
+        <v>110.96</v>
+      </c>
+      <c r="D29" s="3">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F28">
+      <c r="F29">
         <v>23</v>
       </c>
-      <c r="G28" s="1">
+      <c r="G29" s="1">
         <v>0.37037050999999993</v>
       </c>
-      <c r="H28">
+      <c r="H29">
+        <f t="shared" si="10"/>
+        <v>112.83999999999997</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="3"/>
+        <v>119.26999999999998</v>
+      </c>
+      <c r="J29" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+      <c r="K29" s="3">
+        <v>0</v>
+      </c>
+      <c r="L29" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>106.40999999999998</v>
-      </c>
-      <c r="I28">
-        <f t="shared" si="2"/>
-        <v>112.83999999999997</v>
-      </c>
-      <c r="J28" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="K28" s="3">
-        <v>0</v>
-      </c>
-      <c r="L28" s="2" t="str">
-        <f t="shared" si="5"/>
         <v>ok</v>
       </c>
-      <c r="N28" t="s">
-        <v>24</v>
-      </c>
-      <c r="O28">
-        <v>0</v>
-      </c>
-      <c r="P28">
-        <v>0.83</v>
-      </c>
-      <c r="Q28">
-        <v>40.5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>11</v>
-      </c>
-      <c r="B29">
-        <f>VLOOKUP(A29,$N$4:$Q$31,2,FALSE)</f>
-        <v>99.98</v>
-      </c>
-      <c r="C29">
+      <c r="N29" t="s">
+        <v>25</v>
+      </c>
+      <c r="O29">
+        <v>5.34</v>
+      </c>
+      <c r="P29">
+        <v>6.35</v>
+      </c>
+      <c r="Q29">
+        <v>96.19</v>
+      </c>
+      <c r="R29">
+        <v>4.03</v>
+      </c>
+      <c r="S29" s="6">
+        <v>779.57</v>
+      </c>
+      <c r="U29" t="str">
+        <f t="shared" si="7"/>
+        <v>assertEquals(99.98, project.getActivity("Testes Áreas").getStartExecutionTime(), 0.1);</v>
+      </c>
+      <c r="V29" t="str">
+        <f t="shared" si="8"/>
+        <v>assertEquals(110.96, project.getActivity("Testes Áreas").getFinishingTime(), 0.1);</v>
+      </c>
+      <c r="W29" t="str">
+        <f t="shared" si="9"/>
+        <v>assertEquals(0, project.getActivity("Testes Áreas").getErrors(), 0.1);</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23">
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30">
         <f t="shared" si="0"/>
         <v>110.96</v>
       </c>
-      <c r="D29" s="3">
+      <c r="C30">
         <f t="shared" si="1"/>
+        <v>120.28</v>
+      </c>
+      <c r="D30" s="3">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F29">
-        <v>23</v>
-      </c>
-      <c r="G29" s="1">
+      <c r="F30">
+        <v>20</v>
+      </c>
+      <c r="G30" s="1">
         <v>0.37037050999999993</v>
       </c>
-      <c r="H29">
+      <c r="H30">
+        <f t="shared" si="10"/>
+        <v>119.26999999999998</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="3"/>
+        <v>124.86999999999998</v>
+      </c>
+      <c r="J30" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+      <c r="K30" s="3">
+        <v>0</v>
+      </c>
+      <c r="L30" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>112.83999999999997</v>
-      </c>
-      <c r="I29">
-        <f t="shared" si="2"/>
-        <v>119.26999999999998</v>
-      </c>
-      <c r="J29" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="K29" s="3">
-        <v>0</v>
-      </c>
-      <c r="L29" s="2" t="str">
-        <f t="shared" si="5"/>
         <v>ok</v>
       </c>
-      <c r="N29" t="s">
-        <v>25</v>
-      </c>
-      <c r="O29">
-        <v>5.34</v>
-      </c>
-      <c r="P29">
-        <v>6.35</v>
-      </c>
-      <c r="Q29">
-        <v>96.19</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>7</v>
-      </c>
-      <c r="B30">
-        <f>VLOOKUP(A30,$N$4:$Q$31,2,FALSE)</f>
-        <v>110.96</v>
-      </c>
-      <c r="C30">
+      <c r="N30" t="s">
+        <v>26</v>
+      </c>
+      <c r="O30">
+        <v>11.76</v>
+      </c>
+      <c r="P30">
+        <v>18.47</v>
+      </c>
+      <c r="Q30">
+        <v>184.3</v>
+      </c>
+      <c r="R30">
+        <v>26.86</v>
+      </c>
+      <c r="S30" s="6">
+        <v>5197.12</v>
+      </c>
+      <c r="U30" t="str">
+        <f t="shared" si="7"/>
+        <v>assertEquals(110.96, project.getActivity("Testes Professores").getStartExecutionTime(), 0.1);</v>
+      </c>
+      <c r="V30" t="str">
+        <f t="shared" si="8"/>
+        <v>assertEquals(120.28, project.getActivity("Testes Professores").getFinishingTime(), 0.1);</v>
+      </c>
+      <c r="W30" t="str">
+        <f t="shared" si="9"/>
+        <v>assertEquals(0, project.getActivity("Testes Professores").getErrors(), 0.1);</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23">
+      <c r="A31" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31">
         <f t="shared" si="0"/>
         <v>120.28</v>
       </c>
-      <c r="D30" s="3">
+      <c r="C31">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F30">
-        <v>20</v>
-      </c>
-      <c r="G30" s="1">
-        <v>0.37037050999999993</v>
-      </c>
-      <c r="H30">
-        <f t="shared" si="6"/>
-        <v>119.26999999999998</v>
-      </c>
-      <c r="I30">
+        <v>125.67</v>
+      </c>
+      <c r="D31" s="3">
         <f t="shared" si="2"/>
-        <v>124.86999999999998</v>
-      </c>
-      <c r="J30" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="K30" s="3">
-        <v>0</v>
-      </c>
-      <c r="L30" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>ok</v>
-      </c>
-      <c r="N30" t="s">
-        <v>26</v>
-      </c>
-      <c r="O30">
-        <v>11.76</v>
-      </c>
-      <c r="P30">
-        <v>18.47</v>
-      </c>
-      <c r="Q30">
-        <v>184.3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>3</v>
-      </c>
-      <c r="B31">
-        <f>VLOOKUP(A31,$N$4:$Q$31,2,FALSE)</f>
-        <v>120.28</v>
-      </c>
-      <c r="C31">
-        <f t="shared" si="0"/>
-        <v>125.67</v>
-      </c>
-      <c r="D31" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F31">
@@ -2064,22 +2566,22 @@
         <v>0.37037050999999993</v>
       </c>
       <c r="H31">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>124.86999999999998</v>
       </c>
       <c r="I31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>129.90999999999997</v>
       </c>
       <c r="J31" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="K31" s="3">
         <v>0</v>
       </c>
       <c r="L31" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>ok</v>
       </c>
       <c r="N31" t="s">
@@ -2094,8 +2596,36 @@
       <c r="Q31">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="R31">
+        <v>0</v>
+      </c>
+      <c r="S31" s="6">
+        <v>6187.54</v>
+      </c>
+      <c r="U31" t="str">
+        <f t="shared" si="7"/>
+        <v>assertEquals(120.28, project.getActivity("Testes Usuários").getStartExecutionTime(), 0.1);</v>
+      </c>
+      <c r="V31" t="str">
+        <f t="shared" si="8"/>
+        <v>assertEquals(125.67, project.getActivity("Testes Usuários").getFinishingTime(), 0.1);</v>
+      </c>
+      <c r="W31" t="str">
+        <f t="shared" si="9"/>
+        <v>assertEquals(0, project.getActivity("Testes Usuários").getErrors(), 0.1);</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23">
+      <c r="R32" s="6">
+        <f>SUM(R4:R31)</f>
+        <v>262.8</v>
+      </c>
+      <c r="S32" s="6">
+        <f>SUM(S4:S31)</f>
+        <v>79639.34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -2120,7 +2650,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
         <v>40</v>
       </c>
@@ -2131,21 +2661,21 @@
         <v>35</v>
       </c>
       <c r="D34">
-        <f>8*60+4*60*1.5</f>
-        <v>840</v>
+        <f>8*60+2*60*1.2+2*60*1.25</f>
+        <v>774</v>
       </c>
       <c r="E34" t="s">
         <v>36</v>
       </c>
       <c r="F34" s="6">
         <f>B34*D34</f>
-        <v>91786.8</v>
+        <v>84574.98</v>
       </c>
       <c r="G34" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>41</v>
       </c>
@@ -2156,15 +2686,15 @@
         <v>35</v>
       </c>
       <c r="D35">
-        <f>8*60+4*60*1.5</f>
-        <v>840</v>
+        <f>8*60+2*60*1.2+2*60*1.25</f>
+        <v>774</v>
       </c>
       <c r="E35" t="s">
         <v>36</v>
       </c>
       <c r="F35" s="6">
-        <f>B35*D35</f>
-        <v>105562.8</v>
+        <f>(B35-60)*D35+60*D33</f>
+        <v>79628.58</v>
       </c>
       <c r="G35" t="s">
         <v>37</v>

</xml_diff>